<commit_message>
Add second table processing and writing into excel file
</commit_message>
<xml_diff>
--- a/exercise_c/colonnade_currencies.xlsx
+++ b/exercise_c/colonnade_currencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\source\repos\Colonnade_application\exercise_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0336D0-5308-4DFA-A42F-5E3AD0D147D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673051BD-467A-42BF-9548-F1DA0FF3F8EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC2C0307-8B35-4E22-B177-6D13E9B7EFD0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Pénznem</t>
   </si>
@@ -51,7 +51,61 @@
     <t>Forintban kifejezett érték</t>
   </si>
   <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>bolgár leva</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>cseh korona</t>
+  </si>
+  <si>
+    <t>13,35</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>lengyel zloty</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>román lej</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>ukrán hrivnya</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>364,85</t>
+  </si>
+  <si>
     <t>2020. október 16.</t>
+  </si>
+  <si>
+    <t>186,54</t>
+  </si>
+  <si>
+    <t>80,02</t>
+  </si>
+  <si>
+    <t>74,82</t>
+  </si>
+  <si>
+    <t>10,99</t>
   </si>
 </sst>
 </file>
@@ -487,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DFD205-E975-489C-A06D-4F77CE75ADA7}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +555,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -519,6 +573,90 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>